<commit_message>
Eliminated unique for subject slug. Added unique together to school level and slug
</commit_message>
<xml_diff>
--- a/test_data/school_data.xlsx
+++ b/test_data/school_data.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Teachers" sheetId="1" r:id="rId1"/>
+    <sheet name="d" sheetId="3" r:id="rId2"/>
+    <sheet name="Subjects" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>username</t>
   </si>
   <si>
-    <t>captiainamerica</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -111,6 +110,36 @@
   </si>
   <si>
     <t>Rasputin</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>chemistry</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>teacher</t>
+  </si>
+  <si>
+    <t>captainamerica</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>7-a</t>
   </si>
 </sst>
 </file>
@@ -427,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,46 +472,46 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="str">
         <f>CONCATENATE(LOWER(B2),LOWER(D2),"@",E2,".com")</f>
         <v>steverogers@avengers-school.com</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>123456</v>
@@ -490,23 +519,23 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="str">
         <f>CONCATENATE(LOWER(B3),LOWER(D3),"@",E3,".com")</f>
         <v>brucebanner@avengers-school.com</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3">
         <v>123456</v>
@@ -514,23 +543,23 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="str">
         <f>CONCATENATE(LOWER(B4),LOWER(D4),"@",E4,".com")</f>
         <v>anthonystark@avengers-school.com</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4">
         <v>123456</v>
@@ -538,23 +567,23 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
       </c>
       <c r="F5" t="str">
         <f>CONCATENATE(LOWER(B5),LOWER(D5),"@",E5,".com")</f>
         <v>loganhunt@xmen-school.com</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <v>123456</v>
@@ -562,23 +591,23 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" t="str">
         <f>CONCATENATE(LOWER(B6),LOWER(D6),"@",E6,".com")</f>
         <v>ororomonroe@xmen-school.com</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6">
         <v>123456</v>
@@ -586,26 +615,108 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" t="str">
         <f>CONCATENATE(LOWER(B7),LOWER(D7),"@",E7,".com")</f>
         <v>peterrasputin@xmen-school.com</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7">
         <v>123456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>